<commit_message>
added new languages, changed fonts, changed instruction formatting
</commit_message>
<xml_diff>
--- a/Languages/English/Instruction.xlsx
+++ b/Languages/English/Instruction.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pavloviaP\EEGML_RS\restingStatePresentation\Languages\English\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36CD91CF-0C4C-48B6-A2D8-6915D7EF936D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310"/>
+    <workbookView xWindow="390" yWindow="2325" windowWidth="11310" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,13 +30,16 @@
     <t>Instructions</t>
   </si>
   <si>
-    <t>First, processes of the brain will be examined under relaxation conditions. It is therefore very important in this part of the experiment that you relax as much as possible. During the recording of the resting EEG, you will be instructed to open or close your eyes. If you are instructed to open your eyes or to keep them open, please direct your relaxed gaze at the monitor. If you are instructed to close your eyes or to keep them closed, follow this instruction in a relaxed manner. To begin, press the space bar.</t>
+    <t>First, processes of the brain will be examined under relaxation conditions. It is therefore very important in this part of the experiment that you relax as much as possible. 
+During the recording of the resting EEG, you will be instructed to open or close your eyes. If you are instructed to open your eyes or to keep them open, please direct your relaxed gaze at the monitor. 
+If you are instructed to close your eyes or to keep them closed, follow this instruction in a relaxed manner. 
+To begin, press the space bar.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -66,8 +70,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -347,22 +354,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:1" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>